<commit_message>
finished initial problem 7 write up, updated fillNA method so that it is always the mode, finished coding summary tables and exported as excel files, about to code regression analysis
</commit_message>
<xml_diff>
--- a/data_for_regression/df_control_clean.xlsx
+++ b/data_for_regression/df_control_clean.xlsx
@@ -6956,7 +6956,7 @@
         <v>1900</v>
       </c>
       <c r="F145" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G145" t="n">
         <v>0</v>
@@ -21941,7 +21941,7 @@
         <v>1600</v>
       </c>
       <c r="F478" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G478" t="n">
         <v>0</v>
@@ -23066,7 +23066,7 @@
         <v>1900</v>
       </c>
       <c r="F503" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G503" t="n">
         <v>0</v>
@@ -24776,7 +24776,7 @@
         <v>2200</v>
       </c>
       <c r="F541" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G541" t="n">
         <v>0</v>
@@ -24866,7 +24866,7 @@
         <v>1700</v>
       </c>
       <c r="F543" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G543" t="n">
         <v>0</v>
@@ -25406,7 +25406,7 @@
         <v>2300</v>
       </c>
       <c r="F555" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G555" t="n">
         <v>0</v>
@@ -26486,7 +26486,7 @@
         <v>3800</v>
       </c>
       <c r="F579" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G579" t="n">
         <v>0</v>
@@ -28376,7 +28376,7 @@
         <v>1400</v>
       </c>
       <c r="F621" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G621" t="n">
         <v>0</v>
@@ -28601,7 +28601,7 @@
         <v>1600</v>
       </c>
       <c r="F626" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G626" t="n">
         <v>0</v>
@@ -30041,7 +30041,7 @@
         <v>1500</v>
       </c>
       <c r="F658" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G658" t="n">
         <v>0</v>
@@ -31166,7 +31166,7 @@
         <v>1500</v>
       </c>
       <c r="F683" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G683" t="n">
         <v>0</v>
@@ -31301,7 +31301,7 @@
         <v>1500</v>
       </c>
       <c r="F686" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G686" t="n">
         <v>0</v>
@@ -32606,7 +32606,7 @@
         <v>1500</v>
       </c>
       <c r="F715" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G715" t="n">
         <v>0</v>
@@ -32831,7 +32831,7 @@
         <v>1500</v>
       </c>
       <c r="F720" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G720" t="n">
         <v>0</v>
@@ -33821,7 +33821,7 @@
         <v>1500</v>
       </c>
       <c r="F742" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G742" t="n">
         <v>0</v>
@@ -41021,7 +41021,7 @@
         <v>700</v>
       </c>
       <c r="F902" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G902" t="n">
         <v>0</v>

</xml_diff>